<commit_message>
added the required column to indoPacificTemplate_v4.xlsx
</commit_message>
<xml_diff>
--- a/sampledata/indoPacificTemplate_v4.xlsx
+++ b/sampledata/indoPacificTemplate_v4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="232">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -1321,6 +1321,9 @@
   </si>
   <si>
     <t>Barber</t>
+  </si>
+  <si>
+    <t>Annelida</t>
   </si>
 </sst>
 </file>
@@ -1336,6 +1339,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1631,7 +1635,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1775,6 +1779,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="14" borderId="1" xfId="65" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="65" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="65" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="Bad" xfId="65" builtinId="27"/>
@@ -2180,22 +2185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="49" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1640625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="49" customWidth="1"/>
+    <col min="2" max="2" width="41.125" style="49" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="41.125" style="49" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="49" customWidth="1"/>
     <col min="5" max="5" width="46.5" style="49" customWidth="1"/>
     <col min="6" max="6" width="96.5" style="49" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="81.6640625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="81.625" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1">
+    <row r="1" spans="1:7" ht="17" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>123</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" thickTop="1">
+    <row r="2" spans="1:7" ht="31" thickTop="1">
       <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42">
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="15" t="s">
         <v>142</v>
       </c>
@@ -3325,7 +3330,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28">
+    <row r="53" spans="1:7">
       <c r="A53" s="26" t="s">
         <v>211</v>
       </c>
@@ -3384,23 +3389,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC6" sqref="AC6"/>
+      <selection pane="bottomLeft" activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="23.1640625" customWidth="1"/>
+    <col min="7" max="8" width="17.375" customWidth="1"/>
+    <col min="13" max="13" width="23.125" customWidth="1"/>
     <col min="14" max="14" width="13.5" customWidth="1"/>
-    <col min="20" max="20" width="14.1640625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="15.1640625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="25.1640625" customWidth="1"/>
-    <col min="42" max="42" width="12.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="25.125" customWidth="1"/>
+    <col min="42" max="42" width="12.375" customWidth="1"/>
     <col min="48" max="49" width="11.5" customWidth="1"/>
-    <col min="50" max="50" width="15.6640625" customWidth="1"/>
+    <col min="50" max="50" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="7" customFormat="1">
@@ -3656,7 +3661,9 @@
         <v>52</v>
       </c>
       <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
+      <c r="AH2" s="53" t="s">
+        <v>231</v>
+      </c>
       <c r="AI2" s="52"/>
       <c r="AJ2" s="52"/>
       <c r="AK2" s="52"/>
@@ -9723,9 +9730,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>

</xml_diff>